<commit_message>
data_writer.py edited, more input & output files added
</commit_message>
<xml_diff>
--- a/output-files/schedule_5orders.xlsx
+++ b/output-files/schedule_5orders.xlsx
@@ -484,10 +484,10 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>44591.55555555555</v>
+        <v>44576.55555555555</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>44592</v>
+        <v>44577</v>
       </c>
     </row>
     <row r="3">
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44591.55555555555</v>
+        <v>44576.55555555555</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>44592</v>
+        <v>44577</v>
       </c>
     </row>
     <row r="4">
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44591.55555555555</v>
+        <v>44576.55555555555</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>44592</v>
+        <v>44577</v>
       </c>
     </row>
     <row r="5">
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44591.55555555555</v>
+        <v>44576.55555555555</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>44592</v>
+        <v>44577</v>
       </c>
     </row>
     <row r="6">
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>44591.55555555555</v>
+        <v>44576.55555555555</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>44592</v>
+        <v>44577</v>
       </c>
     </row>
     <row r="7">
@@ -614,10 +614,10 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>44591.55555555555</v>
+        <v>44576.55555555555</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>44592</v>
+        <v>44577</v>
       </c>
     </row>
     <row r="8">
@@ -640,10 +640,10 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>44588.33263888889</v>
+        <v>44571.47986111111</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>44588.61875</v>
+        <v>44571.76597222222</v>
       </c>
     </row>
     <row r="9">
@@ -666,10 +666,10 @@
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>44587.55833333333</v>
+        <v>44573.97638888889</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>44587.84444444445</v>
+        <v>44574.2625</v>
       </c>
     </row>
     <row r="10">
@@ -678,7 +678,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>139</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -692,10 +692,10 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>44589.10694444444</v>
+        <v>44574.28333333333</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>44589.39305555556</v>
+        <v>44574.56736111111</v>
       </c>
     </row>
     <row r="11">
@@ -718,10 +718,10 @@
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>44589.84722222222</v>
+        <v>44574.84722222222</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>44590.16666666666</v>
+        <v>44575.16666666666</v>
       </c>
     </row>
     <row r="12">
@@ -744,10 +744,10 @@
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>44586.2369047619</v>
+        <v>44574.57569444444</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>44586.52301587301</v>
+        <v>44574.86180555556</v>
       </c>
     </row>
     <row r="13">
@@ -756,7 +756,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>139</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -770,10 +770,10 @@
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>44589.88055555556</v>
+        <v>44574.88263888889</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>44590.16666666666</v>
+        <v>44575.16666666666</v>
       </c>
     </row>
     <row r="14">
@@ -796,10 +796,10 @@
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>44587.31041666667</v>
+        <v>44570.45763888889</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>44587.62986111111</v>
+        <v>44570.77708333333</v>
       </c>
     </row>
     <row r="15">
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>44586.53611111111</v>
+        <v>44572.00625</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>44586.85555555556</v>
+        <v>44572.32569444444</v>
       </c>
     </row>
     <row r="16">
@@ -848,10 +848,10 @@
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>44588.08472222222</v>
+        <v>44571.23194444444</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>44588.40416666667</v>
+        <v>44571.55138888889</v>
       </c>
     </row>
     <row r="17">
@@ -874,10 +874,10 @@
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>44588.09375</v>
+        <v>44573.09375</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>44588.45833333334</v>
+        <v>44573.45833333334</v>
       </c>
     </row>
     <row r="18">
@@ -900,10 +900,10 @@
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>44585.21468253968</v>
+        <v>44573.55347222222</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>44585.53412698412</v>
+        <v>44573.87291666667</v>
       </c>
     </row>
     <row r="19">
@@ -926,10 +926,10 @@
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>44588.85833333333</v>
+        <v>44572.77986111111</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>44589.17777777778</v>
+        <v>44573.09930555556</v>
       </c>
     </row>
     <row r="20">
@@ -952,10 +952,10 @@
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>44585.64027777778</v>
+        <v>44568.7875</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>44585.92152777778</v>
+        <v>44569.06875</v>
       </c>
     </row>
     <row r="21">
@@ -978,10 +978,10 @@
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>44584.86597222222</v>
+        <v>44570.33611111111</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>44585.14722222222</v>
+        <v>44570.61736111111</v>
       </c>
     </row>
     <row r="22">
@@ -1004,10 +1004,10 @@
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>44586.41458333333</v>
+        <v>44569.56180555555</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>44586.69583333333</v>
+        <v>44569.84305555555</v>
       </c>
     </row>
     <row r="23">
@@ -1030,10 +1030,10 @@
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>44586.59241071429</v>
+        <v>44571.59241071429</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>44587.06254960317</v>
+        <v>44572.06254960317</v>
       </c>
     </row>
     <row r="24">
@@ -1056,10 +1056,10 @@
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>44583.54523809523</v>
+        <v>44571.88402777778</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>44583.82579365079</v>
+        <v>44572.16458333333</v>
       </c>
     </row>
     <row r="25">
@@ -1082,10 +1082,10 @@
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>44587.18888888889</v>
+        <v>44571.11041666667</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>44587.46944444445</v>
+        <v>44571.39097222222</v>
       </c>
     </row>
     <row r="26">
@@ -1108,10 +1108,10 @@
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>44583.4</v>
+        <v>44567.32152777778</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>44583.67847222222</v>
+        <v>44567.6</v>
       </c>
     </row>
     <row r="27">
@@ -1160,10 +1160,10 @@
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>44582.73963293651</v>
+        <v>44566.66116071428</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>44583.01810515873</v>
+        <v>44566.9396329365</v>
       </c>
     </row>
     <row r="29">
@@ -1238,10 +1238,10 @@
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>44581.09454365079</v>
+        <v>44565.33606150793</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>44581.37301587301</v>
+        <v>44565.61453373015</v>
       </c>
     </row>
     <row r="32">
@@ -1264,10 +1264,10 @@
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>44566.32078373015</v>
+        <v>44568.30625</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>44566.59925595237</v>
+        <v>44568.58472222222</v>
       </c>
     </row>
     <row r="33">
@@ -1290,10 +1290,10 @@
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>44582.07926587301</v>
+        <v>44569.64444444444</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>44582.35773809523</v>
+        <v>44569.92291666667</v>
       </c>
     </row>
     <row r="34">
@@ -1316,10 +1316,10 @@
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>44566.98115079365</v>
+        <v>44568.96661706348</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>44567.25962301587</v>
+        <v>44569.24508928571</v>
       </c>
     </row>
     <row r="35">
@@ -1342,10 +1342,10 @@
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>44582.0333829365</v>
+        <v>44565.95491071428</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>44582.32366071428</v>
+        <v>44566.24518849206</v>
       </c>
     </row>
     <row r="36">
@@ -1394,10 +1394,10 @@
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>44563.96944444445</v>
+        <v>44562</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>44564.25972222222</v>
+        <v>44562.29027777778</v>
       </c>
     </row>
     <row r="38">
@@ -1472,10 +1472,10 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>44579.72792658729</v>
+        <v>44563.96944444445</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>44580.01820436507</v>
+        <v>44564.25972222222</v>
       </c>
     </row>
     <row r="41">
@@ -1498,10 +1498,10 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>44564.95416666667</v>
+        <v>44566.9396329365</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>44565.24444444444</v>
+        <v>44567.22991071428</v>
       </c>
     </row>
     <row r="42">
@@ -1524,10 +1524,10 @@
         </is>
       </c>
       <c r="E42" s="2" t="n">
-        <v>44580.71264880952</v>
+        <v>44568.27782738095</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>44581.00292658729</v>
+        <v>44568.56810515872</v>
       </c>
     </row>
     <row r="43">
@@ -1550,10 +1550,10 @@
         </is>
       </c>
       <c r="E43" s="2" t="n">
-        <v>44562</v>
+        <v>44564.95416666667</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>44562.29027777778</v>
+        <v>44565.24444444444</v>
       </c>
     </row>
     <row r="44">

</xml_diff>